<commit_message>
add note about use of bearings
</commit_message>
<xml_diff>
--- a/Bill_of_Material/Bill of materials (Arduino model) .xlsx
+++ b/Bill_of_Material/Bill of materials (Arduino model) .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bldfr\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bldfr\OneDrive\Documenti\GitHub\pyo\Bill_of_Material\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEB5C261-5BB9-4A0B-BE49-BBBE1F1C7C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A831ADC-45E5-46D2-B7B3-19BD1F4FD35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>What I need to reproduce Pyo platform with Arduino</t>
   </si>
@@ -158,12 +158,18 @@
   <si>
     <t>https://www.amazon.com/BTF-LIGHTING-Individual-Addressable-Flexible-Controllers/dp/B088BTXHRG/ref=sr_1_6?crid=1SEOWVTWHJX6Y&amp;keywords=rgb%2Bled%2Bmatrix&amp;qid=1655724288&amp;sprefix=rgb%2Bled%2Bmatri%2Caps%2C215&amp;sr=8-6&amp;th=1</t>
   </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>I suggest to use 2 overlapping bearings or modify the 3d model (it is difficult to find one 12mm high but with 10mm hole)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -222,6 +228,12 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -250,7 +262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -316,6 +328,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -539,14 +554,14 @@
   <dimension ref="A1:AA1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="4" max="4" width="39.44140625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" customWidth="1"/>
+    <col min="5" max="5" width="81.21875" customWidth="1"/>
     <col min="8" max="8" width="32.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -592,7 +607,9 @@
       <c r="D2" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="7"/>
@@ -995,7 +1012,9 @@
       <c r="D13" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="32" t="s">
+        <v>43</v>
+      </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
@@ -29873,5 +29892,6 @@
     <hyperlink ref="D19" r:id="rId16" xr:uid="{ED50E478-7B8D-472F-8434-408E02E312F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>